<commit_message>
Mise à jour du code et de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -1,25 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6832561-9FEC-4059-BDEF-6855632293CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Auteur</t>
+  </si>
+  <si>
+    <t>Débout du journal</t>
+  </si>
+  <si>
+    <t>Projet</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>I-CT 431</t>
+  </si>
+  <si>
+    <t>Monteiro Rui</t>
+  </si>
+  <si>
+    <t>Bataille Navale</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +67,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -45,12 +89,182 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +544,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="O1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="15" max="15" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="15:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="7"/>
+    </row>
+    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="11">
+        <f ca="1">TODAY()</f>
+        <v>44267</v>
+      </c>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="15:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>